<commit_message>
rewriting group func( not working yet)
</commit_message>
<xml_diff>
--- a/ImageIndex.xlsx
+++ b/ImageIndex.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\PycharmProjects\Mercenaries-Hearthstone-game-bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E27CD5-DE65-457B-81AD-3444FA662BDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFBBB7BA-CF23-47B9-93DE-BF9690E21986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="28800" windowHeight="15330" xr2:uid="{F6B23E98-3404-4A1A-B6BD-EC022861F775}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="120" windowWidth="28800" windowHeight="15330" xr2:uid="{F6B23E98-3404-4A1A-B6BD-EC022861F775}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t xml:space="preserve"> 'continue'</t>
   </si>
@@ -238,6 +238,15 @@
   </si>
   <si>
     <t>startbat</t>
+  </si>
+  <si>
+    <t>cords-search</t>
+  </si>
+  <si>
+    <t>30lvl1</t>
+  </si>
+  <si>
+    <t>30lvl2</t>
   </si>
 </sst>
 </file>
@@ -295,7 +304,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -303,6 +312,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,7 +630,7 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,6 +1013,9 @@
       <c r="E19" s="3">
         <v>17</v>
       </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -1020,6 +1033,9 @@
       <c r="E20" s="3">
         <v>18</v>
       </c>
+      <c r="F20" s="7">
+        <v>303</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
@@ -1037,6 +1053,9 @@
       <c r="E21" s="3">
         <v>19</v>
       </c>
+      <c r="F21" s="7" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
@@ -1054,6 +1073,9 @@
       <c r="E22" s="3">
         <v>20</v>
       </c>
+      <c r="F22" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
@@ -1071,6 +1093,7 @@
       <c r="E23" s="3">
         <v>21</v>
       </c>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3">

</xml_diff>